<commit_message>
passage m1 a m2
</commit_message>
<xml_diff>
--- a/liste_etu_postM1.xlsx
+++ b/liste_etu_postM1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>Nom</t>
   </si>
@@ -23,6 +23,12 @@
     <t>Prénom</t>
   </si>
   <si>
+    <t>Promo</t>
+  </si>
+  <si>
+    <t>TypeAnnée</t>
+  </si>
+  <si>
     <t>Parcours</t>
   </si>
   <si>
@@ -45,6 +51,99 @@
   </si>
   <si>
     <t>NomTA</t>
+  </si>
+  <si>
+    <t>ABBE</t>
+  </si>
+  <si>
+    <t>TRISTAN</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>GPhy</t>
+  </si>
+  <si>
+    <t>apprentissage</t>
+  </si>
+  <si>
+    <t>SANOFI</t>
+  </si>
+  <si>
+    <t>Gentilly (94)</t>
+  </si>
+  <si>
+    <t>BELLOCQ</t>
+  </si>
+  <si>
+    <t>GENIET</t>
+  </si>
+  <si>
+    <t>KONE</t>
+  </si>
+  <si>
+    <t>YACOUBA</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>pro</t>
+  </si>
+  <si>
+    <t>LABORATOIRE XLIM</t>
+  </si>
+  <si>
+    <t>Poitiers</t>
+  </si>
+  <si>
+    <t>BOURDON</t>
+  </si>
+  <si>
+    <t>URRUTY</t>
+  </si>
+  <si>
+    <t>MONTBULEAU--GENTELET</t>
+  </si>
+  <si>
+    <t>TITOUAN</t>
+  </si>
+  <si>
+    <t>MAAT PHARMA</t>
+  </si>
+  <si>
+    <t>Lyon</t>
+  </si>
+  <si>
+    <t>BERGÉ</t>
+  </si>
+  <si>
+    <t>0617421317</t>
+  </si>
+  <si>
+    <t>NIGGEL</t>
+  </si>
+  <si>
+    <t>THIBAULT</t>
+  </si>
+  <si>
+    <t>stage</t>
+  </si>
+  <si>
+    <t>EVALU CONSEIL</t>
+  </si>
+  <si>
+    <t>Paris / à distance</t>
+  </si>
+  <si>
+    <t>MONNé</t>
+  </si>
+  <si>
+    <t>0615097890</t>
+  </si>
+  <si>
+    <t>SAVANY</t>
   </si>
 </sst>
 </file>
@@ -384,7 +483,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -392,7 +491,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,6 +521,166 @@
       </c>
       <c r="J1" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>2025</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>2025</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>2025</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5">
+        <v>2025</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>2025</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix tab domi + excel
</commit_message>
<xml_diff>
--- a/liste_etu_postM1.xlsx
+++ b/liste_etu_postM1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>Nom</t>
   </si>
@@ -53,10 +53,10 @@
     <t>NomTA</t>
   </si>
   <si>
-    <t>ABBE</t>
-  </si>
-  <si>
-    <t>TRISTAN</t>
+    <t>MONTBULEAU--GENTELET</t>
+  </si>
+  <si>
+    <t>TITOUAN</t>
   </si>
   <si>
     <t>M2</t>
@@ -65,85 +65,22 @@
     <t>GPhy</t>
   </si>
   <si>
-    <t>apprentissage</t>
-  </si>
-  <si>
-    <t>SANOFI</t>
-  </si>
-  <si>
-    <t>Gentilly (94)</t>
-  </si>
-  <si>
-    <t>BELLOCQ</t>
-  </si>
-  <si>
-    <t>GENIET</t>
-  </si>
-  <si>
-    <t>KONE</t>
-  </si>
-  <si>
-    <t>YACOUBA</t>
-  </si>
-  <si>
-    <t>M1</t>
-  </si>
-  <si>
-    <t>pro</t>
-  </si>
-  <si>
-    <t>LABORATOIRE XLIM</t>
-  </si>
-  <si>
-    <t>Poitiers</t>
-  </si>
-  <si>
-    <t>BOURDON</t>
+    <t>stage</t>
+  </si>
+  <si>
+    <t>MAAT PHARMA</t>
+  </si>
+  <si>
+    <t>Lyon</t>
+  </si>
+  <si>
+    <t>BERGÉ</t>
+  </si>
+  <si>
+    <t>0617421317</t>
   </si>
   <si>
     <t>URRUTY</t>
-  </si>
-  <si>
-    <t>MONTBULEAU--GENTELET</t>
-  </si>
-  <si>
-    <t>TITOUAN</t>
-  </si>
-  <si>
-    <t>MAAT PHARMA</t>
-  </si>
-  <si>
-    <t>Lyon</t>
-  </si>
-  <si>
-    <t>BERGÉ</t>
-  </si>
-  <si>
-    <t>0617421317</t>
-  </si>
-  <si>
-    <t>NIGGEL</t>
-  </si>
-  <si>
-    <t>THIBAULT</t>
-  </si>
-  <si>
-    <t>stage</t>
-  </si>
-  <si>
-    <t>EVALU CONSEIL</t>
-  </si>
-  <si>
-    <t>Paris / à distance</t>
-  </si>
-  <si>
-    <t>MONNé</t>
-  </si>
-  <si>
-    <t>0615097890</t>
-  </si>
-  <si>
-    <t>SAVANY</t>
   </si>
 </sst>
 </file>
@@ -483,7 +420,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -557,130 +494,11 @@
       <c r="J2" t="s">
         <v>19</v>
       </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
       <c r="L2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
         <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3">
-        <v>2025</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4">
-        <v>2025</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5">
-        <v>2025</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" t="s">
-        <v>41</v>
-      </c>
-      <c r="L5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6">
-        <v>2025</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout date deb et fin
</commit_message>
<xml_diff>
--- a/liste_etu_postM1.xlsx
+++ b/liste_etu_postM1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
   <si>
     <t>Nom</t>
   </si>
@@ -53,19 +53,52 @@
     <t>NomTA</t>
   </si>
   <si>
+    <t>DateDébut</t>
+  </si>
+  <si>
+    <t>DateFin</t>
+  </si>
+  <si>
+    <t>ABBE</t>
+  </si>
+  <si>
+    <t>TRISTAN</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>GPhy</t>
+  </si>
+  <si>
+    <t>stage</t>
+  </si>
+  <si>
+    <t>SANOFI</t>
+  </si>
+  <si>
+    <t>Gentilly (94)</t>
+  </si>
+  <si>
+    <t>BELLOCQ</t>
+  </si>
+  <si>
+    <t>GENIET</t>
+  </si>
+  <si>
+    <t>2024-05-21</t>
+  </si>
+  <si>
+    <t>2024-08-23</t>
+  </si>
+  <si>
     <t>MONTBULEAU--GENTELET</t>
   </si>
   <si>
     <t>TITOUAN</t>
   </si>
   <si>
-    <t>M2</t>
-  </si>
-  <si>
-    <t>GPhy</t>
-  </si>
-  <si>
-    <t>stage</t>
+    <t>apprentissage</t>
   </si>
   <si>
     <t>MAAT PHARMA</t>
@@ -81,6 +114,48 @@
   </si>
   <si>
     <t>URRUTY</t>
+  </si>
+  <si>
+    <t>2024-08-31</t>
+  </si>
+  <si>
+    <t>SEVILLA</t>
+  </si>
+  <si>
+    <t>MATHIEU</t>
+  </si>
+  <si>
+    <t>LABVANTAGE</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>MAIRE</t>
+  </si>
+  <si>
+    <t>+(33)6 74.01.53.57</t>
+  </si>
+  <si>
+    <t>SOCHARD</t>
+  </si>
+  <si>
+    <t>OPHELIE</t>
+  </si>
+  <si>
+    <t>AMEXIO</t>
+  </si>
+  <si>
+    <t>Paris, Montpellier, Lille et Nantes</t>
+  </si>
+  <si>
+    <t>01 81 69 86 00</t>
+  </si>
+  <si>
+    <t>2024-05-27</t>
+  </si>
+  <si>
+    <t>2024-08-16</t>
   </si>
 </sst>
 </file>
@@ -420,7 +495,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,7 +503,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,40 +540,172 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>2025</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>2025</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4">
+        <v>2025</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" t="s">
-        <v>21</v>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>2025</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>